<commit_message>
looked up an additional marker region, changes to some graphs
</commit_message>
<xml_diff>
--- a/data/Gene_annotations/Germination/Chr5H_3_mrna_list.xlsx
+++ b/data/Gene_annotations/Germination/Chr5H_3_mrna_list.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl\git\BarleyGermination-KK\data\Gene_annotations\Germination\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8862CE04-ABDC-4FEB-A462-D5DDD8977CF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506DDC23-21C7-4BC3-925E-B79800A6D5A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11880" yWindow="-11985" windowWidth="14400" windowHeight="7815"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chr5H_3_mrna" sheetId="1" r:id="rId1"/>
@@ -931,7 +931,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1821,11 +1821,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6037,10 +6037,10 @@
     <sortCondition ref="B2:B73"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="G60" r:id="rId1"/>
-    <hyperlink ref="I61" r:id="rId2" display="https://doi.org/10.1111/j.1399-3054.2009.01338.x"/>
-    <hyperlink ref="I66" r:id="rId3"/>
-    <hyperlink ref="I4" r:id="rId4" display="https://dx.doi.org/10.1105%2Ftpc.108.061374"/>
+    <hyperlink ref="G60" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="I61" r:id="rId2" display="https://doi.org/10.1111/j.1399-3054.2009.01338.x" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="I66" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="I4" r:id="rId4" display="https://dx.doi.org/10.1105%2Ftpc.108.061374" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>